<commit_message>
set color and merge col export excel
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/test.xlsx
+++ b/src/storage/app/excel-exporter/templates/test.xlsx
@@ -41,55 +41,98 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Phòng: {division} – Cở sở: {branch}</t>
+      <t xml:space="preserve">Phòng: {division} – Cơ sở: {branch}</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ghi chú: 
-Nghỉ 1 ngày có phép F 
+    <t xml:space="preserve">Stt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vị trí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[month]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thực công
+{work}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ký tên
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">{sign}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[[date]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[number]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[fullName]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[position]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[values]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[totalWork]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[sign]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ghi chú:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nghỉ 1 ngày có phép F {note}
 Nghỉ 1/2 ngày có phép F/2                   Có phép được tính khi: 
 Nghỉ 1 ngày không phép K                   - Có buổi đơn xin phép và được chấp thuận
 Nghỉ 1/2 ngày không phép K/2            - Buổi nghỉ đột xuất có lý do được chấp thuận</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tên</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vị trí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[[month]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thực công</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ký tên</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[[date]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[number]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[fullName]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[position]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[[values]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[totalWork]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[sign]</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -101,8 +144,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-    <numFmt numFmtId="166" formatCode="hh:mm"/>
+    <numFmt numFmtId="165" formatCode="hh:mm"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -141,20 +184,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -162,9 +200,16 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -247,7 +292,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,23 +300,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,43 +320,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,9 +387,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1572480</xdr:colOff>
+      <xdr:colOff>1571400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -358,12 +403,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="13320"/>
-          <a:ext cx="1856160" cy="809280"/>
+          <a:ext cx="1855080" cy="808200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -378,13 +423,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.92"/>
@@ -392,7 +437,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -409,139 +454,123 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="107.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="9" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" customFormat="false" ht="67.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" customFormat="false" ht="11.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="20" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="20" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>